<commit_message>
update general + ponencia
</commit_message>
<xml_diff>
--- a/operac-variables.xlsx
+++ b/operac-variables.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/ciortiz1_uc_cl/Documents/Investigación y proyectos/[COBA] Determinantes de la Cohesión Barrial/dse-cob-tesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uccl0-my.sharepoint.com/personal/ciortiz1_uc_cl/Documents/Investigación y proyectos/[COBA] Cohesión Barrial/dse-cob-tesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="13_ncr:1_{AE3C510C-7BAF-41EF-B6C5-949A98C5563A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{740DA874-2EAE-4284-9D5A-C1831FB4C3A8}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="13_ncr:1_{AE3C510C-7BAF-41EF-B6C5-949A98C5563A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87E60353-E748-4ECE-A196-D0D09DA7E018}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="propuesta-ieut" sheetId="12" r:id="rId1"/>
-    <sheet name="co-ba" sheetId="13" r:id="rId2"/>
+    <sheet name="propuesta-demosal" sheetId="15" r:id="rId2"/>
+    <sheet name="Hoja4" sheetId="17" r:id="rId3"/>
+    <sheet name="co-ba" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="112">
   <si>
     <t>Dimensión</t>
   </si>
@@ -341,6 +343,36 @@
   </si>
   <si>
     <t xml:space="preserve"> social</t>
+  </si>
+  <si>
+    <t>Índice de theil</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Grado de acuerdo: Me siento integrado/a en este barrio</t>
+  </si>
+  <si>
+    <t>Afectiva</t>
+  </si>
+  <si>
+    <t>Indice de theil</t>
+  </si>
+  <si>
+    <t>Subjetiva</t>
+  </si>
+  <si>
+    <t>Objetiva</t>
+  </si>
+  <si>
+    <t>Seguridad barrial</t>
+  </si>
+  <si>
+    <t>Satisfacción barrial</t>
+  </si>
+  <si>
+    <t>Reputación barrial</t>
   </si>
 </sst>
 </file>
@@ -752,7 +784,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -816,6 +848,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -831,58 +872,52 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E0AD90-AC84-4EEE-91C8-E57592F10B31}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1198,13 +1233,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="25" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1215,47 +1250,47 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="27"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="27"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
       <c r="D4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="23"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="26" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="27"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="23"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A7" s="27"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
       <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1264,8 +1299,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1277,92 +1312,92 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A9" s="27"/>
-      <c r="B9" s="22" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="26" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="27"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
       <c r="D10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="23"/>
+      <c r="E10" s="26"/>
     </row>
     <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A11" s="27"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="27"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
       <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="23"/>
+      <c r="E12" s="26"/>
     </row>
     <row r="13" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A13" s="27"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
       <c r="D13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="27"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
       <c r="D14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="23"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A15" s="27"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="27"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
       <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="23"/>
+      <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A17" s="27"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
@@ -1374,8 +1409,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A18" s="27"/>
-      <c r="B18" s="22" t="s">
+      <c r="A18" s="24"/>
+      <c r="B18" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1389,8 +1424,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A19" s="27"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1402,10 +1437,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="30" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
@@ -1419,8 +1454,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="27"/>
-      <c r="B21" s="28"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="30"/>
       <c r="C21" s="5" t="s">
         <v>57</v>
       </c>
@@ -1432,8 +1467,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="27"/>
-      <c r="B22" s="28"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="30"/>
       <c r="C22" s="5" t="s">
         <v>60</v>
       </c>
@@ -1445,8 +1480,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A23" s="27"/>
-      <c r="B23" s="28"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="5" t="s">
         <v>61</v>
       </c>
@@ -1458,8 +1493,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A24" s="27"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="5" t="s">
         <v>64</v>
       </c>
@@ -1471,8 +1506,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A25" s="27"/>
-      <c r="B25" s="28" t="s">
+      <c r="A25" s="24"/>
+      <c r="B25" s="30" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="5" t="s">
@@ -1486,8 +1521,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="5" t="s">
         <v>71</v>
       </c>
@@ -1499,8 +1534,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="30"/>
       <c r="C27" s="5" t="s">
         <v>72</v>
       </c>
@@ -1512,8 +1547,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
+      <c r="A28" s="24"/>
+      <c r="B28" s="30"/>
       <c r="C28" s="5" t="s">
         <v>73</v>
       </c>
@@ -1525,33 +1560,33 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28" t="s">
+      <c r="A29" s="24"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30" t="s">
         <v>76</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="23" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A31" s="27"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="24"/>
+      <c r="B31" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="27" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -1562,9 +1597,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="42" x14ac:dyDescent="0.35">
-      <c r="A32" s="27"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
       <c r="D32" s="7" t="s">
         <v>82</v>
       </c>
@@ -1573,9 +1608,9 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A33" s="27"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
       <c r="D33" s="7" t="s">
         <v>83</v>
       </c>
@@ -1584,9 +1619,9 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A34" s="27"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="7" t="s">
         <v>84</v>
       </c>
@@ -1595,8 +1630,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
-      <c r="B35" s="25"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="5" t="s">
         <v>85</v>
       </c>
@@ -1608,8 +1643,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A36" s="27"/>
-      <c r="B36" s="26"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="5" t="s">
         <v>87</v>
       </c>
@@ -1622,12 +1657,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A2:A19"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C2:C7"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
     <mergeCell ref="C31:C34"/>
     <mergeCell ref="A20:A36"/>
     <mergeCell ref="B31:B36"/>
@@ -1641,6 +1670,12 @@
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B25:B30"/>
     <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A2:A19"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C7"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1648,11 +1683,173 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B80FD8-33EB-48D2-BD47-73C8750D8065}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A6" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28" x14ac:dyDescent="0.35">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="29"/>
+      <c r="B12" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D8B81E-35BA-46BE-8517-0A069689EC74}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3DF786-94B4-42D0-BA01-F27D0E2CA803}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1662,7 +1859,7 @@
     <col min="3" max="3" width="46.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="29" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1676,11 +1873,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="45" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1690,45 +1887,48 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3" s="31"/>
-      <c r="B3" s="34"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="36"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="31"/>
-      <c r="B4" s="34"/>
+    <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="36"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="37"/>
-    </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A5" s="31"/>
-      <c r="B5" s="34"/>
+      <c r="D4" s="32"/>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="36"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="31"/>
-      <c r="B6" s="34"/>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="36"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="37"/>
-    </row>
-    <row r="7" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31"/>
-      <c r="B7" s="35"/>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="36"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="17" t="s">
         <v>28</v>
       </c>
@@ -1736,169 +1936,174 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.35">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="36"/>
       <c r="B8" s="19" t="s">
         <v>91</v>
       </c>
       <c r="C8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="32"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="42"/>
       <c r="B9" s="20" t="s">
         <v>92</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="37"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A10" s="40" t="s">
+      <c r="D9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="38" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="31"/>
-      <c r="B11" s="34"/>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="36"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="37"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A12" s="31"/>
-      <c r="B12" s="34"/>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A12" s="36"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34"/>
+    <row r="13" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="36"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="37"/>
-    </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A14" s="31"/>
-      <c r="B14" s="34"/>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A14" s="36"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="31"/>
-      <c r="B15" s="34"/>
+    <row r="15" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="36"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="37"/>
-    </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A16" s="31"/>
-      <c r="B16" s="34"/>
+      <c r="D15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+      <c r="A16" s="36"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D16" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="37"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="31"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="36"/>
       <c r="B18" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D18" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="32"/>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="42"/>
       <c r="B19" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="37"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="32"/>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.35">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="38" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="31" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="31"/>
-      <c r="B21" s="35"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="37"/>
-    </row>
-    <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="31"/>
+      <c r="D21" s="32"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="36"/>
       <c r="B22" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="C22" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="41"/>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="37"/>
       <c r="B23" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
     </row>
     <row r="24" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D8:D9"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
@@ -1912,11 +2117,6 @@
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D8:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>